<commit_message>
Updated data for wk5-middle
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\wzmnz_game_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D83B298-B1CE-44F6-B18C-A89001FD7FBE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4A44F6D-3CD4-4D0E-BFED-C3716CF06788}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FB48B202-EBC4-4DF3-96AB-433FACB95B1A}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1449" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1927" uniqueCount="179">
   <si>
     <t>阵容</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -698,6 +698,35 @@
   </si>
   <si>
     <t>质量</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>扶桑群雄刺</t>
+  </si>
+  <si>
+    <t>弟弟蜀</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CW</t>
+  </si>
+  <si>
+    <t>RW侠</t>
+  </si>
+  <si>
+    <t>次手手</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>扶桑刺</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>水晶</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>长城战</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1075,10 +1104,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EB2E6C9-7049-424A-A14B-939D1CD70783}">
-  <dimension ref="A1:M241"/>
+  <dimension ref="A1:M321"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" topLeftCell="A280" workbookViewId="0">
+      <selection activeCell="H299" sqref="H299"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -10968,6 +10997,3286 @@
         <v>5</v>
       </c>
       <c r="M241" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="242" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A242">
+        <v>1</v>
+      </c>
+      <c r="B242" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C242" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D242" t="s">
+        <v>12</v>
+      </c>
+      <c r="E242" t="s">
+        <v>27</v>
+      </c>
+      <c r="F242" s="2">
+        <v>85</v>
+      </c>
+      <c r="G242" s="3">
+        <v>197</v>
+      </c>
+      <c r="H242" s="3">
+        <v>22</v>
+      </c>
+      <c r="I242" s="3">
+        <v>4</v>
+      </c>
+      <c r="J242">
+        <v>5</v>
+      </c>
+      <c r="K242" t="s">
+        <v>38</v>
+      </c>
+      <c r="L242">
+        <v>1</v>
+      </c>
+      <c r="M242" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="243" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A243">
+        <v>2</v>
+      </c>
+      <c r="B243" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C243" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D243" t="s">
+        <v>41</v>
+      </c>
+      <c r="E243" t="s">
+        <v>62</v>
+      </c>
+      <c r="F243" s="2">
+        <v>76</v>
+      </c>
+      <c r="G243" s="3">
+        <v>69</v>
+      </c>
+      <c r="H243" s="3">
+        <v>17</v>
+      </c>
+      <c r="I243" s="3">
+        <v>9</v>
+      </c>
+      <c r="J243">
+        <v>5</v>
+      </c>
+      <c r="K243" t="s">
+        <v>39</v>
+      </c>
+      <c r="L243">
+        <v>1</v>
+      </c>
+      <c r="M243" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="244" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A244">
+        <v>3</v>
+      </c>
+      <c r="B244" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C244" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D244" t="s">
+        <v>11</v>
+      </c>
+      <c r="E244" t="s">
+        <v>24</v>
+      </c>
+      <c r="F244" s="2">
+        <v>90</v>
+      </c>
+      <c r="G244" s="3">
+        <v>113</v>
+      </c>
+      <c r="H244" s="3">
+        <v>14</v>
+      </c>
+      <c r="I244" s="3">
+        <v>12</v>
+      </c>
+      <c r="J244">
+        <v>5</v>
+      </c>
+      <c r="K244" t="s">
+        <v>39</v>
+      </c>
+      <c r="L244">
+        <v>1</v>
+      </c>
+      <c r="M244" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="245" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A245">
+        <v>4</v>
+      </c>
+      <c r="B245" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C245" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D245" t="s">
+        <v>9</v>
+      </c>
+      <c r="E245" t="s">
+        <v>21</v>
+      </c>
+      <c r="F245" s="2">
+        <v>69</v>
+      </c>
+      <c r="G245" s="3">
+        <v>98</v>
+      </c>
+      <c r="H245" s="3">
+        <v>15</v>
+      </c>
+      <c r="I245" s="3">
+        <v>9</v>
+      </c>
+      <c r="J245">
+        <v>5</v>
+      </c>
+      <c r="K245" t="s">
+        <v>39</v>
+      </c>
+      <c r="L245">
+        <v>1</v>
+      </c>
+      <c r="M245" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="246" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A246">
+        <v>5</v>
+      </c>
+      <c r="B246" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C246" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D246" t="s">
+        <v>7</v>
+      </c>
+      <c r="E246" t="s">
+        <v>148</v>
+      </c>
+      <c r="F246" s="2">
+        <v>60</v>
+      </c>
+      <c r="G246" s="3">
+        <v>89</v>
+      </c>
+      <c r="H246" s="3">
+        <v>14</v>
+      </c>
+      <c r="I246" s="3">
+        <v>9</v>
+      </c>
+      <c r="J246">
+        <v>5</v>
+      </c>
+      <c r="K246" t="s">
+        <v>39</v>
+      </c>
+      <c r="L246">
+        <v>1</v>
+      </c>
+      <c r="M246" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="247" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A247">
+        <v>6</v>
+      </c>
+      <c r="B247" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C247" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D247" t="s">
+        <v>11</v>
+      </c>
+      <c r="E247" t="s">
+        <v>24</v>
+      </c>
+      <c r="F247" s="2">
+        <v>63</v>
+      </c>
+      <c r="G247" s="3">
+        <v>101</v>
+      </c>
+      <c r="H247" s="3">
+        <v>12</v>
+      </c>
+      <c r="I247" s="3">
+        <v>10</v>
+      </c>
+      <c r="J247">
+        <v>5</v>
+      </c>
+      <c r="K247" t="s">
+        <v>39</v>
+      </c>
+      <c r="L247">
+        <v>1</v>
+      </c>
+      <c r="M247" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="248" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A248">
+        <v>7</v>
+      </c>
+      <c r="B248" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C248" s="1">
+        <v>52</v>
+      </c>
+      <c r="D248" t="s">
+        <v>11</v>
+      </c>
+      <c r="E248" t="s">
+        <v>21</v>
+      </c>
+      <c r="F248" s="2">
+        <v>72</v>
+      </c>
+      <c r="G248" s="3">
+        <v>52</v>
+      </c>
+      <c r="H248" s="3">
+        <v>11</v>
+      </c>
+      <c r="I248" s="3">
+        <v>10</v>
+      </c>
+      <c r="J248">
+        <v>5</v>
+      </c>
+      <c r="K248" t="s">
+        <v>39</v>
+      </c>
+      <c r="L248">
+        <v>1</v>
+      </c>
+      <c r="M248" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="249" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A249">
+        <v>8</v>
+      </c>
+      <c r="B249" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C249" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D249" t="s">
+        <v>7</v>
+      </c>
+      <c r="E249" t="s">
+        <v>13</v>
+      </c>
+      <c r="F249" s="2">
+        <v>58</v>
+      </c>
+      <c r="G249" s="3">
+        <v>28</v>
+      </c>
+      <c r="H249" s="3">
+        <v>9</v>
+      </c>
+      <c r="I249" s="3">
+        <v>9</v>
+      </c>
+      <c r="J249">
+        <v>5</v>
+      </c>
+      <c r="K249" t="s">
+        <v>39</v>
+      </c>
+      <c r="L249">
+        <v>1</v>
+      </c>
+      <c r="M249" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="250" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A250">
+        <v>1</v>
+      </c>
+      <c r="B250" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C250" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D250" t="s">
+        <v>8</v>
+      </c>
+      <c r="E250" t="s">
+        <v>148</v>
+      </c>
+      <c r="F250" s="2">
+        <v>120</v>
+      </c>
+      <c r="G250" s="3">
+        <v>223</v>
+      </c>
+      <c r="H250" s="3">
+        <v>26</v>
+      </c>
+      <c r="I250" s="3">
+        <v>5</v>
+      </c>
+      <c r="J250">
+        <v>5</v>
+      </c>
+      <c r="K250" t="s">
+        <v>39</v>
+      </c>
+      <c r="L250">
+        <v>2</v>
+      </c>
+      <c r="M250" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="251" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A251">
+        <v>2</v>
+      </c>
+      <c r="B251" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C251" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D251" t="s">
+        <v>41</v>
+      </c>
+      <c r="E251" t="s">
+        <v>62</v>
+      </c>
+      <c r="F251" s="2">
+        <v>93</v>
+      </c>
+      <c r="G251" s="3">
+        <v>111</v>
+      </c>
+      <c r="H251" s="3">
+        <v>20</v>
+      </c>
+      <c r="I251" s="3">
+        <v>11</v>
+      </c>
+      <c r="J251">
+        <v>5</v>
+      </c>
+      <c r="K251" t="s">
+        <v>39</v>
+      </c>
+      <c r="L251">
+        <v>2</v>
+      </c>
+      <c r="M251" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="252" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A252">
+        <v>3</v>
+      </c>
+      <c r="B252" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C252" s="1">
+        <v>52</v>
+      </c>
+      <c r="D252" t="s">
+        <v>6</v>
+      </c>
+      <c r="E252" t="s">
+        <v>18</v>
+      </c>
+      <c r="F252" s="2">
+        <v>81</v>
+      </c>
+      <c r="G252" s="3">
+        <v>100</v>
+      </c>
+      <c r="H252" s="3">
+        <v>16</v>
+      </c>
+      <c r="I252" s="3">
+        <v>12</v>
+      </c>
+      <c r="J252">
+        <v>5</v>
+      </c>
+      <c r="K252" t="s">
+        <v>39</v>
+      </c>
+      <c r="L252">
+        <v>2</v>
+      </c>
+      <c r="M252" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="253" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A253">
+        <v>4</v>
+      </c>
+      <c r="B253" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C253" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D253" t="s">
+        <v>12</v>
+      </c>
+      <c r="E253" t="s">
+        <v>27</v>
+      </c>
+      <c r="F253" s="2">
+        <v>69</v>
+      </c>
+      <c r="G253" s="3">
+        <v>69</v>
+      </c>
+      <c r="H253" s="3">
+        <v>14</v>
+      </c>
+      <c r="I253" s="3">
+        <v>12</v>
+      </c>
+      <c r="J253">
+        <v>5</v>
+      </c>
+      <c r="K253" t="s">
+        <v>39</v>
+      </c>
+      <c r="L253">
+        <v>2</v>
+      </c>
+      <c r="M253" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="254" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A254">
+        <v>5</v>
+      </c>
+      <c r="B254" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C254" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D254" t="s">
+        <v>41</v>
+      </c>
+      <c r="E254" t="s">
+        <v>34</v>
+      </c>
+      <c r="F254" s="2">
+        <v>80</v>
+      </c>
+      <c r="G254" s="3">
+        <v>85</v>
+      </c>
+      <c r="H254" s="3">
+        <v>14</v>
+      </c>
+      <c r="I254" s="3">
+        <v>12</v>
+      </c>
+      <c r="J254">
+        <v>5</v>
+      </c>
+      <c r="K254" t="s">
+        <v>39</v>
+      </c>
+      <c r="L254">
+        <v>2</v>
+      </c>
+      <c r="M254" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="255" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A255">
+        <v>6</v>
+      </c>
+      <c r="B255" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C255" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D255" t="s">
+        <v>7</v>
+      </c>
+      <c r="E255" t="s">
+        <v>21</v>
+      </c>
+      <c r="F255" s="2">
+        <v>73</v>
+      </c>
+      <c r="G255" s="3">
+        <v>62</v>
+      </c>
+      <c r="H255" s="3">
+        <v>13</v>
+      </c>
+      <c r="I255" s="3">
+        <v>11</v>
+      </c>
+      <c r="J255">
+        <v>5</v>
+      </c>
+      <c r="K255" t="s">
+        <v>39</v>
+      </c>
+      <c r="L255">
+        <v>2</v>
+      </c>
+      <c r="M255" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="256" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A256">
+        <v>7</v>
+      </c>
+      <c r="B256" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C256" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D256" t="s">
+        <v>12</v>
+      </c>
+      <c r="E256" t="s">
+        <v>58</v>
+      </c>
+      <c r="F256" s="2">
+        <v>58</v>
+      </c>
+      <c r="G256" s="3">
+        <v>115</v>
+      </c>
+      <c r="H256" s="3">
+        <v>15</v>
+      </c>
+      <c r="I256" s="3">
+        <v>8</v>
+      </c>
+      <c r="J256">
+        <v>5</v>
+      </c>
+      <c r="K256" t="s">
+        <v>39</v>
+      </c>
+      <c r="L256">
+        <v>2</v>
+      </c>
+      <c r="M256" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="257" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A257">
+        <v>8</v>
+      </c>
+      <c r="B257" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C257" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D257" t="s">
+        <v>9</v>
+      </c>
+      <c r="E257" t="s">
+        <v>13</v>
+      </c>
+      <c r="F257" s="2">
+        <v>41</v>
+      </c>
+      <c r="G257" s="3">
+        <v>24</v>
+      </c>
+      <c r="H257" s="3">
+        <v>8</v>
+      </c>
+      <c r="I257" s="3">
+        <v>10</v>
+      </c>
+      <c r="J257">
+        <v>5</v>
+      </c>
+      <c r="K257" t="s">
+        <v>39</v>
+      </c>
+      <c r="L257">
+        <v>2</v>
+      </c>
+      <c r="M257" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="258" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A258">
+        <v>1</v>
+      </c>
+      <c r="B258" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C258" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="D258" t="s">
+        <v>7</v>
+      </c>
+      <c r="E258" t="s">
+        <v>13</v>
+      </c>
+      <c r="F258" s="2">
+        <v>67</v>
+      </c>
+      <c r="G258" s="3">
+        <v>261</v>
+      </c>
+      <c r="H258" s="3">
+        <v>22</v>
+      </c>
+      <c r="I258" s="3">
+        <v>4</v>
+      </c>
+      <c r="J258">
+        <v>5</v>
+      </c>
+      <c r="K258" t="s">
+        <v>39</v>
+      </c>
+      <c r="L258">
+        <v>3</v>
+      </c>
+      <c r="M258" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="259" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A259">
+        <v>2</v>
+      </c>
+      <c r="B259" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C259" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D259" t="s">
+        <v>11</v>
+      </c>
+      <c r="E259" t="s">
+        <v>151</v>
+      </c>
+      <c r="F259" s="2">
+        <v>92</v>
+      </c>
+      <c r="G259" s="3">
+        <v>99</v>
+      </c>
+      <c r="H259" s="3">
+        <v>18</v>
+      </c>
+      <c r="I259" s="3">
+        <v>8</v>
+      </c>
+      <c r="J259">
+        <v>5</v>
+      </c>
+      <c r="K259" t="s">
+        <v>39</v>
+      </c>
+      <c r="L259">
+        <v>3</v>
+      </c>
+      <c r="M259" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="260" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A260">
+        <v>3</v>
+      </c>
+      <c r="B260" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C260" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D260" t="s">
+        <v>41</v>
+      </c>
+      <c r="E260" t="s">
+        <v>62</v>
+      </c>
+      <c r="F260" s="2">
+        <v>55</v>
+      </c>
+      <c r="G260" s="3">
+        <v>59</v>
+      </c>
+      <c r="H260" s="3">
+        <v>14</v>
+      </c>
+      <c r="I260" s="3">
+        <v>10</v>
+      </c>
+      <c r="J260">
+        <v>5</v>
+      </c>
+      <c r="K260" t="s">
+        <v>39</v>
+      </c>
+      <c r="L260">
+        <v>3</v>
+      </c>
+      <c r="M260" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="261" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A261">
+        <v>4</v>
+      </c>
+      <c r="B261" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C261" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D261" t="s">
+        <v>7</v>
+      </c>
+      <c r="E261" t="s">
+        <v>21</v>
+      </c>
+      <c r="F261" s="2">
+        <v>83</v>
+      </c>
+      <c r="G261" s="3">
+        <v>80</v>
+      </c>
+      <c r="H261" s="3">
+        <v>12</v>
+      </c>
+      <c r="I261" s="3">
+        <v>12</v>
+      </c>
+      <c r="J261">
+        <v>5</v>
+      </c>
+      <c r="K261" t="s">
+        <v>39</v>
+      </c>
+      <c r="L261">
+        <v>3</v>
+      </c>
+      <c r="M261" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="262" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A262">
+        <v>5</v>
+      </c>
+      <c r="B262" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C262" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D262" t="s">
+        <v>59</v>
+      </c>
+      <c r="E262" t="s">
+        <v>27</v>
+      </c>
+      <c r="F262" s="2">
+        <v>72</v>
+      </c>
+      <c r="G262" s="3">
+        <v>65</v>
+      </c>
+      <c r="H262" s="3">
+        <v>13</v>
+      </c>
+      <c r="I262" s="3">
+        <v>10</v>
+      </c>
+      <c r="J262">
+        <v>5</v>
+      </c>
+      <c r="K262" t="s">
+        <v>39</v>
+      </c>
+      <c r="L262">
+        <v>3</v>
+      </c>
+      <c r="M262" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="263" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A263">
+        <v>6</v>
+      </c>
+      <c r="B263" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C263" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D263" t="s">
+        <v>59</v>
+      </c>
+      <c r="E263" t="s">
+        <v>27</v>
+      </c>
+      <c r="F263" s="2">
+        <v>59</v>
+      </c>
+      <c r="G263" s="3">
+        <v>62</v>
+      </c>
+      <c r="H263" s="3">
+        <v>12</v>
+      </c>
+      <c r="I263" s="3">
+        <v>10</v>
+      </c>
+      <c r="J263">
+        <v>5</v>
+      </c>
+      <c r="K263" t="s">
+        <v>39</v>
+      </c>
+      <c r="L263">
+        <v>3</v>
+      </c>
+      <c r="M263" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="264" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A264">
+        <v>7</v>
+      </c>
+      <c r="B264" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C264" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D264" t="s">
+        <v>12</v>
+      </c>
+      <c r="E264" t="s">
+        <v>58</v>
+      </c>
+      <c r="F264" s="2">
+        <v>49</v>
+      </c>
+      <c r="G264" s="3">
+        <v>56</v>
+      </c>
+      <c r="H264" s="3">
+        <v>12</v>
+      </c>
+      <c r="I264" s="3">
+        <v>9</v>
+      </c>
+      <c r="J264">
+        <v>5</v>
+      </c>
+      <c r="K264" t="s">
+        <v>39</v>
+      </c>
+      <c r="L264">
+        <v>3</v>
+      </c>
+      <c r="M264" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="265" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A265">
+        <v>8</v>
+      </c>
+      <c r="B265" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C265" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D265" t="s">
+        <v>41</v>
+      </c>
+      <c r="E265" t="s">
+        <v>62</v>
+      </c>
+      <c r="F265" s="2">
+        <v>40</v>
+      </c>
+      <c r="G265" s="3">
+        <v>39</v>
+      </c>
+      <c r="H265" s="3">
+        <v>11</v>
+      </c>
+      <c r="I265" s="3">
+        <v>8</v>
+      </c>
+      <c r="J265">
+        <v>5</v>
+      </c>
+      <c r="K265" t="s">
+        <v>39</v>
+      </c>
+      <c r="L265">
+        <v>3</v>
+      </c>
+      <c r="M265" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="266" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A266">
+        <v>1</v>
+      </c>
+      <c r="B266" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C266" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D266" t="s">
+        <v>41</v>
+      </c>
+      <c r="E266" t="s">
+        <v>62</v>
+      </c>
+      <c r="F266" s="2">
+        <v>78</v>
+      </c>
+      <c r="G266" s="3">
+        <v>138</v>
+      </c>
+      <c r="H266" s="3">
+        <v>27</v>
+      </c>
+      <c r="I266" s="3">
+        <v>1</v>
+      </c>
+      <c r="J266">
+        <v>5</v>
+      </c>
+      <c r="K266" t="s">
+        <v>39</v>
+      </c>
+      <c r="L266">
+        <v>4</v>
+      </c>
+      <c r="M266" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="267" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A267">
+        <v>2</v>
+      </c>
+      <c r="B267" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C267" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D267" t="s">
+        <v>59</v>
+      </c>
+      <c r="E267" t="s">
+        <v>148</v>
+      </c>
+      <c r="F267" s="2">
+        <v>95</v>
+      </c>
+      <c r="G267" s="3">
+        <v>88</v>
+      </c>
+      <c r="H267" s="3">
+        <v>15</v>
+      </c>
+      <c r="I267" s="3">
+        <v>13</v>
+      </c>
+      <c r="J267">
+        <v>5</v>
+      </c>
+      <c r="K267" t="s">
+        <v>39</v>
+      </c>
+      <c r="L267">
+        <v>4</v>
+      </c>
+      <c r="M267" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="268" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A268">
+        <v>3</v>
+      </c>
+      <c r="B268" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C268" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D268" t="s">
+        <v>52</v>
+      </c>
+      <c r="E268" t="s">
+        <v>24</v>
+      </c>
+      <c r="F268" s="2">
+        <v>86</v>
+      </c>
+      <c r="G268" s="3">
+        <v>140</v>
+      </c>
+      <c r="H268" s="3">
+        <v>12</v>
+      </c>
+      <c r="I268" s="3">
+        <v>15</v>
+      </c>
+      <c r="J268">
+        <v>5</v>
+      </c>
+      <c r="K268" t="s">
+        <v>39</v>
+      </c>
+      <c r="L268">
+        <v>4</v>
+      </c>
+      <c r="M268" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="269" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A269">
+        <v>4</v>
+      </c>
+      <c r="B269" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C269" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D269" t="s">
+        <v>7</v>
+      </c>
+      <c r="E269" t="s">
+        <v>13</v>
+      </c>
+      <c r="F269" s="2">
+        <v>79</v>
+      </c>
+      <c r="G269" s="3">
+        <v>95</v>
+      </c>
+      <c r="H269" s="3">
+        <v>12</v>
+      </c>
+      <c r="I269" s="3">
+        <v>12</v>
+      </c>
+      <c r="J269">
+        <v>5</v>
+      </c>
+      <c r="K269" t="s">
+        <v>39</v>
+      </c>
+      <c r="L269">
+        <v>4</v>
+      </c>
+      <c r="M269" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="270" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A270">
+        <v>5</v>
+      </c>
+      <c r="B270" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C270" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D270" t="s">
+        <v>52</v>
+      </c>
+      <c r="E270" t="s">
+        <v>24</v>
+      </c>
+      <c r="F270" s="2">
+        <v>73</v>
+      </c>
+      <c r="G270" s="3">
+        <v>85</v>
+      </c>
+      <c r="H270" s="3">
+        <v>12</v>
+      </c>
+      <c r="I270" s="3">
+        <v>10</v>
+      </c>
+      <c r="J270">
+        <v>5</v>
+      </c>
+      <c r="K270" t="s">
+        <v>39</v>
+      </c>
+      <c r="L270">
+        <v>4</v>
+      </c>
+      <c r="M270" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="271" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A271">
+        <v>6</v>
+      </c>
+      <c r="B271" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C271" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D271" t="s">
+        <v>8</v>
+      </c>
+      <c r="E271" t="s">
+        <v>34</v>
+      </c>
+      <c r="F271" s="2">
+        <v>69</v>
+      </c>
+      <c r="G271" s="3">
+        <v>72</v>
+      </c>
+      <c r="H271" s="3">
+        <v>14</v>
+      </c>
+      <c r="I271" s="3">
+        <v>8</v>
+      </c>
+      <c r="J271">
+        <v>5</v>
+      </c>
+      <c r="K271" t="s">
+        <v>39</v>
+      </c>
+      <c r="L271">
+        <v>4</v>
+      </c>
+      <c r="M271" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="272" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A272">
+        <v>7</v>
+      </c>
+      <c r="B272" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C272" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="D272" t="s">
+        <v>9</v>
+      </c>
+      <c r="E272" t="s">
+        <v>172</v>
+      </c>
+      <c r="F272" s="2">
+        <v>62</v>
+      </c>
+      <c r="G272" s="3">
+        <v>72</v>
+      </c>
+      <c r="H272" s="3">
+        <v>14</v>
+      </c>
+      <c r="I272" s="3">
+        <v>7</v>
+      </c>
+      <c r="J272">
+        <v>5</v>
+      </c>
+      <c r="K272" t="s">
+        <v>39</v>
+      </c>
+      <c r="L272">
+        <v>4</v>
+      </c>
+      <c r="M272" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="273" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A273">
+        <v>8</v>
+      </c>
+      <c r="B273" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C273" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D273" t="s">
+        <v>9</v>
+      </c>
+      <c r="E273" t="s">
+        <v>34</v>
+      </c>
+      <c r="F273" s="2">
+        <v>47</v>
+      </c>
+      <c r="G273" s="3">
+        <v>44</v>
+      </c>
+      <c r="H273" s="3">
+        <v>10</v>
+      </c>
+      <c r="I273" s="3">
+        <v>8</v>
+      </c>
+      <c r="J273">
+        <v>5</v>
+      </c>
+      <c r="K273" t="s">
+        <v>39</v>
+      </c>
+      <c r="L273">
+        <v>4</v>
+      </c>
+      <c r="M273" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="274" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A274">
+        <v>1</v>
+      </c>
+      <c r="B274" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C274" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D274" t="s">
+        <v>41</v>
+      </c>
+      <c r="E274" t="s">
+        <v>149</v>
+      </c>
+      <c r="F274" s="2">
+        <v>115</v>
+      </c>
+      <c r="G274" s="3">
+        <v>218</v>
+      </c>
+      <c r="H274" s="3">
+        <v>24</v>
+      </c>
+      <c r="I274" s="3">
+        <v>10</v>
+      </c>
+      <c r="J274">
+        <v>5</v>
+      </c>
+      <c r="K274" t="s">
+        <v>39</v>
+      </c>
+      <c r="L274">
+        <v>5</v>
+      </c>
+      <c r="M274" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="275" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A275">
+        <v>2</v>
+      </c>
+      <c r="B275" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C275" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D275" t="s">
+        <v>12</v>
+      </c>
+      <c r="E275" t="s">
+        <v>27</v>
+      </c>
+      <c r="F275" s="2">
+        <v>112</v>
+      </c>
+      <c r="G275" s="3">
+        <v>179</v>
+      </c>
+      <c r="H275" s="3">
+        <v>24</v>
+      </c>
+      <c r="I275" s="3">
+        <v>10</v>
+      </c>
+      <c r="J275">
+        <v>5</v>
+      </c>
+      <c r="K275" t="s">
+        <v>39</v>
+      </c>
+      <c r="L275">
+        <v>5</v>
+      </c>
+      <c r="M275" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="276" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A276">
+        <v>3</v>
+      </c>
+      <c r="B276" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C276" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D276" t="s">
+        <v>9</v>
+      </c>
+      <c r="E276" t="s">
+        <v>148</v>
+      </c>
+      <c r="F276" s="2">
+        <v>99</v>
+      </c>
+      <c r="G276" s="3">
+        <v>111</v>
+      </c>
+      <c r="H276" s="3">
+        <v>21</v>
+      </c>
+      <c r="I276" s="3">
+        <v>10</v>
+      </c>
+      <c r="J276">
+        <v>5</v>
+      </c>
+      <c r="K276" t="s">
+        <v>39</v>
+      </c>
+      <c r="L276">
+        <v>5</v>
+      </c>
+      <c r="M276" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="277" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A277">
+        <v>4</v>
+      </c>
+      <c r="B277" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C277" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="D277" t="s">
+        <v>11</v>
+      </c>
+      <c r="E277" t="s">
+        <v>21</v>
+      </c>
+      <c r="F277" s="2">
+        <v>79</v>
+      </c>
+      <c r="G277" s="3">
+        <v>83</v>
+      </c>
+      <c r="H277" s="3">
+        <v>17</v>
+      </c>
+      <c r="I277" s="3">
+        <v>12</v>
+      </c>
+      <c r="J277">
+        <v>5</v>
+      </c>
+      <c r="K277" t="s">
+        <v>39</v>
+      </c>
+      <c r="L277">
+        <v>5</v>
+      </c>
+      <c r="M277" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="278" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A278">
+        <v>5</v>
+      </c>
+      <c r="B278" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C278" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D278" t="s">
+        <v>9</v>
+      </c>
+      <c r="E278" t="s">
+        <v>34</v>
+      </c>
+      <c r="F278" s="2">
+        <v>70</v>
+      </c>
+      <c r="G278" s="3">
+        <v>107</v>
+      </c>
+      <c r="H278" s="3">
+        <v>14</v>
+      </c>
+      <c r="I278" s="3">
+        <v>10</v>
+      </c>
+      <c r="J278">
+        <v>5</v>
+      </c>
+      <c r="K278" t="s">
+        <v>39</v>
+      </c>
+      <c r="L278">
+        <v>5</v>
+      </c>
+      <c r="M278" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="279" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A279">
+        <v>6</v>
+      </c>
+      <c r="B279" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C279" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D279" t="s">
+        <v>41</v>
+      </c>
+      <c r="E279" t="s">
+        <v>62</v>
+      </c>
+      <c r="F279" s="2">
+        <v>45</v>
+      </c>
+      <c r="G279" s="3">
+        <v>46</v>
+      </c>
+      <c r="H279" s="3">
+        <v>14</v>
+      </c>
+      <c r="I279" s="3">
+        <v>8</v>
+      </c>
+      <c r="J279">
+        <v>5</v>
+      </c>
+      <c r="K279" t="s">
+        <v>39</v>
+      </c>
+      <c r="L279">
+        <v>5</v>
+      </c>
+      <c r="M279" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="280" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A280">
+        <v>7</v>
+      </c>
+      <c r="B280" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C280" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D280" t="s">
+        <v>52</v>
+      </c>
+      <c r="E280" t="s">
+        <v>24</v>
+      </c>
+      <c r="F280" s="2">
+        <v>57</v>
+      </c>
+      <c r="G280" s="3">
+        <v>38</v>
+      </c>
+      <c r="H280" s="3">
+        <v>8</v>
+      </c>
+      <c r="I280" s="3">
+        <v>11</v>
+      </c>
+      <c r="J280">
+        <v>5</v>
+      </c>
+      <c r="K280" t="s">
+        <v>39</v>
+      </c>
+      <c r="L280">
+        <v>5</v>
+      </c>
+      <c r="M280" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="281" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A281">
+        <v>8</v>
+      </c>
+      <c r="B281" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C281" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D281" t="s">
+        <v>12</v>
+      </c>
+      <c r="E281" t="s">
+        <v>58</v>
+      </c>
+      <c r="F281" s="2">
+        <v>41</v>
+      </c>
+      <c r="G281" s="3">
+        <v>51</v>
+      </c>
+      <c r="H281" s="3">
+        <v>9</v>
+      </c>
+      <c r="I281" s="3">
+        <v>9</v>
+      </c>
+      <c r="J281">
+        <v>5</v>
+      </c>
+      <c r="K281" t="s">
+        <v>39</v>
+      </c>
+      <c r="L281">
+        <v>5</v>
+      </c>
+      <c r="M281" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="282" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A282">
+        <v>1</v>
+      </c>
+      <c r="B282" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C282" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D282" t="s">
+        <v>11</v>
+      </c>
+      <c r="E282" t="s">
+        <v>148</v>
+      </c>
+      <c r="F282" s="2">
+        <v>97</v>
+      </c>
+      <c r="G282" s="3">
+        <v>194</v>
+      </c>
+      <c r="H282" s="3">
+        <v>23</v>
+      </c>
+      <c r="I282" s="3">
+        <v>5</v>
+      </c>
+      <c r="J282">
+        <v>5</v>
+      </c>
+      <c r="K282" t="s">
+        <v>65</v>
+      </c>
+      <c r="L282">
+        <v>1</v>
+      </c>
+      <c r="M282" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="283" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A283">
+        <v>2</v>
+      </c>
+      <c r="B283" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C283" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D283" t="s">
+        <v>41</v>
+      </c>
+      <c r="E283" t="s">
+        <v>149</v>
+      </c>
+      <c r="F283" s="2">
+        <v>92</v>
+      </c>
+      <c r="G283" s="3">
+        <v>140</v>
+      </c>
+      <c r="H283" s="3">
+        <v>21</v>
+      </c>
+      <c r="I283" s="3">
+        <v>7</v>
+      </c>
+      <c r="J283">
+        <v>5</v>
+      </c>
+      <c r="K283" t="s">
+        <v>65</v>
+      </c>
+      <c r="L283">
+        <v>1</v>
+      </c>
+      <c r="M283" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="284" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A284">
+        <v>3</v>
+      </c>
+      <c r="B284" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C284" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D284" t="s">
+        <v>7</v>
+      </c>
+      <c r="E284" t="s">
+        <v>13</v>
+      </c>
+      <c r="F284" s="2">
+        <v>96</v>
+      </c>
+      <c r="G284" s="3">
+        <v>100</v>
+      </c>
+      <c r="H284" s="3">
+        <v>14</v>
+      </c>
+      <c r="I284" s="3">
+        <v>12</v>
+      </c>
+      <c r="J284">
+        <v>5</v>
+      </c>
+      <c r="K284" t="s">
+        <v>65</v>
+      </c>
+      <c r="L284">
+        <v>1</v>
+      </c>
+      <c r="M284" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="285" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A285">
+        <v>4</v>
+      </c>
+      <c r="B285" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C285" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D285" t="s">
+        <v>11</v>
+      </c>
+      <c r="E285" t="s">
+        <v>27</v>
+      </c>
+      <c r="F285" s="2">
+        <v>73</v>
+      </c>
+      <c r="G285" s="3">
+        <v>119</v>
+      </c>
+      <c r="H285" s="3">
+        <v>17</v>
+      </c>
+      <c r="I285" s="3">
+        <v>9</v>
+      </c>
+      <c r="J285">
+        <v>5</v>
+      </c>
+      <c r="K285" t="s">
+        <v>65</v>
+      </c>
+      <c r="L285">
+        <v>1</v>
+      </c>
+      <c r="M285" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="286" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A286">
+        <v>5</v>
+      </c>
+      <c r="B286" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="C286" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="D286" t="s">
+        <v>7</v>
+      </c>
+      <c r="E286" t="s">
+        <v>18</v>
+      </c>
+      <c r="F286" s="2">
+        <v>85</v>
+      </c>
+      <c r="G286" s="3">
+        <v>68</v>
+      </c>
+      <c r="H286" s="3">
+        <v>12</v>
+      </c>
+      <c r="I286" s="3">
+        <v>11</v>
+      </c>
+      <c r="J286">
+        <v>5</v>
+      </c>
+      <c r="K286" t="s">
+        <v>65</v>
+      </c>
+      <c r="L286">
+        <v>1</v>
+      </c>
+      <c r="M286" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="287" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A287">
+        <v>6</v>
+      </c>
+      <c r="B287" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C287" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D287" t="s">
+        <v>7</v>
+      </c>
+      <c r="E287" t="s">
+        <v>156</v>
+      </c>
+      <c r="F287" s="2">
+        <v>68</v>
+      </c>
+      <c r="G287" s="3">
+        <v>51</v>
+      </c>
+      <c r="H287" s="3">
+        <v>13</v>
+      </c>
+      <c r="I287" s="3">
+        <v>10</v>
+      </c>
+      <c r="J287">
+        <v>5</v>
+      </c>
+      <c r="K287" t="s">
+        <v>65</v>
+      </c>
+      <c r="L287">
+        <v>1</v>
+      </c>
+      <c r="M287" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="288" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A288">
+        <v>7</v>
+      </c>
+      <c r="B288" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C288" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D288" t="s">
+        <v>41</v>
+      </c>
+      <c r="E288" t="s">
+        <v>62</v>
+      </c>
+      <c r="F288" s="2">
+        <v>51</v>
+      </c>
+      <c r="G288" s="3">
+        <v>54</v>
+      </c>
+      <c r="H288" s="3">
+        <v>12</v>
+      </c>
+      <c r="I288" s="3">
+        <v>10</v>
+      </c>
+      <c r="J288">
+        <v>5</v>
+      </c>
+      <c r="K288" t="s">
+        <v>65</v>
+      </c>
+      <c r="L288">
+        <v>1</v>
+      </c>
+      <c r="M288" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="289" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A289">
+        <v>8</v>
+      </c>
+      <c r="B289" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C289" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="D289" t="s">
+        <v>41</v>
+      </c>
+      <c r="E289" t="s">
+        <v>62</v>
+      </c>
+      <c r="F289" s="2">
+        <v>61</v>
+      </c>
+      <c r="G289" s="3">
+        <v>48</v>
+      </c>
+      <c r="H289" s="3">
+        <v>9</v>
+      </c>
+      <c r="I289" s="3">
+        <v>12</v>
+      </c>
+      <c r="J289">
+        <v>5</v>
+      </c>
+      <c r="K289" t="s">
+        <v>65</v>
+      </c>
+      <c r="L289">
+        <v>1</v>
+      </c>
+      <c r="M289" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="290" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A290">
+        <v>1</v>
+      </c>
+      <c r="B290" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C290" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D290" t="s">
+        <v>6</v>
+      </c>
+      <c r="E290" t="s">
+        <v>18</v>
+      </c>
+      <c r="F290" s="2">
+        <v>147</v>
+      </c>
+      <c r="G290" s="3">
+        <v>194</v>
+      </c>
+      <c r="H290" s="3">
+        <v>25</v>
+      </c>
+      <c r="I290" s="3">
+        <v>7</v>
+      </c>
+      <c r="J290">
+        <v>5</v>
+      </c>
+      <c r="K290" t="s">
+        <v>65</v>
+      </c>
+      <c r="L290">
+        <v>2</v>
+      </c>
+      <c r="M290" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="291" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A291">
+        <v>2</v>
+      </c>
+      <c r="B291" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C291" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="D291" t="s">
+        <v>52</v>
+      </c>
+      <c r="E291" t="s">
+        <v>24</v>
+      </c>
+      <c r="F291" s="2">
+        <v>116</v>
+      </c>
+      <c r="G291" s="3">
+        <v>220</v>
+      </c>
+      <c r="H291" s="3">
+        <v>23</v>
+      </c>
+      <c r="I291" s="3">
+        <v>9</v>
+      </c>
+      <c r="J291">
+        <v>5</v>
+      </c>
+      <c r="K291" t="s">
+        <v>65</v>
+      </c>
+      <c r="L291">
+        <v>2</v>
+      </c>
+      <c r="M291" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="292" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A292">
+        <v>3</v>
+      </c>
+      <c r="B292" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C292" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D292" t="s">
+        <v>9</v>
+      </c>
+      <c r="E292" t="s">
+        <v>172</v>
+      </c>
+      <c r="F292" s="2">
+        <v>98</v>
+      </c>
+      <c r="G292" s="3">
+        <v>127</v>
+      </c>
+      <c r="H292" s="3">
+        <v>21</v>
+      </c>
+      <c r="I292" s="3">
+        <v>10</v>
+      </c>
+      <c r="J292">
+        <v>5</v>
+      </c>
+      <c r="K292" t="s">
+        <v>65</v>
+      </c>
+      <c r="L292">
+        <v>2</v>
+      </c>
+      <c r="M292" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="293" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A293">
+        <v>4</v>
+      </c>
+      <c r="B293" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C293" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D293" t="s">
+        <v>9</v>
+      </c>
+      <c r="E293" t="s">
+        <v>21</v>
+      </c>
+      <c r="F293" s="2">
+        <v>98</v>
+      </c>
+      <c r="G293" s="3">
+        <v>127</v>
+      </c>
+      <c r="H293" s="3">
+        <v>21</v>
+      </c>
+      <c r="I293" s="3">
+        <v>10</v>
+      </c>
+      <c r="J293">
+        <v>5</v>
+      </c>
+      <c r="K293" t="s">
+        <v>65</v>
+      </c>
+      <c r="L293">
+        <v>2</v>
+      </c>
+      <c r="M293" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="294" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A294">
+        <v>5</v>
+      </c>
+      <c r="B294" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C294" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D294" t="s">
+        <v>41</v>
+      </c>
+      <c r="E294" t="s">
+        <v>62</v>
+      </c>
+      <c r="F294" s="2">
+        <v>69</v>
+      </c>
+      <c r="G294" s="3">
+        <v>90</v>
+      </c>
+      <c r="H294" s="3">
+        <v>16</v>
+      </c>
+      <c r="I294" s="3">
+        <v>10</v>
+      </c>
+      <c r="J294">
+        <v>5</v>
+      </c>
+      <c r="K294" t="s">
+        <v>65</v>
+      </c>
+      <c r="L294">
+        <v>2</v>
+      </c>
+      <c r="M294" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="295" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A295">
+        <v>6</v>
+      </c>
+      <c r="B295" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C295" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D295" t="s">
+        <v>7</v>
+      </c>
+      <c r="E295" t="s">
+        <v>94</v>
+      </c>
+      <c r="F295" s="2">
+        <v>67</v>
+      </c>
+      <c r="G295" s="3">
+        <v>34</v>
+      </c>
+      <c r="H295" s="3">
+        <v>11</v>
+      </c>
+      <c r="I295" s="3">
+        <v>11</v>
+      </c>
+      <c r="J295">
+        <v>5</v>
+      </c>
+      <c r="K295" t="s">
+        <v>65</v>
+      </c>
+      <c r="L295">
+        <v>2</v>
+      </c>
+      <c r="M295" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="296" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A296">
+        <v>7</v>
+      </c>
+      <c r="B296" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C296" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D296" t="s">
+        <v>59</v>
+      </c>
+      <c r="E296" t="s">
+        <v>21</v>
+      </c>
+      <c r="F296" s="2">
+        <v>64</v>
+      </c>
+      <c r="G296" s="3">
+        <v>43</v>
+      </c>
+      <c r="H296" s="3">
+        <v>9</v>
+      </c>
+      <c r="I296" s="3">
+        <v>13</v>
+      </c>
+      <c r="J296">
+        <v>5</v>
+      </c>
+      <c r="K296" t="s">
+        <v>65</v>
+      </c>
+      <c r="L296">
+        <v>2</v>
+      </c>
+      <c r="M296" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="297" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A297">
+        <v>8</v>
+      </c>
+      <c r="B297" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C297" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D297" t="s">
+        <v>11</v>
+      </c>
+      <c r="E297" t="s">
+        <v>176</v>
+      </c>
+      <c r="F297" s="2">
+        <v>52</v>
+      </c>
+      <c r="G297" s="3">
+        <v>11</v>
+      </c>
+      <c r="H297" s="3">
+        <v>6</v>
+      </c>
+      <c r="I297" s="3">
+        <v>11</v>
+      </c>
+      <c r="J297">
+        <v>5</v>
+      </c>
+      <c r="K297" t="s">
+        <v>65</v>
+      </c>
+      <c r="L297">
+        <v>2</v>
+      </c>
+      <c r="M297" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="298" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A298">
+        <v>1</v>
+      </c>
+      <c r="B298" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C298" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D298" t="s">
+        <v>9</v>
+      </c>
+      <c r="E298" t="s">
+        <v>18</v>
+      </c>
+      <c r="F298" s="2">
+        <v>141</v>
+      </c>
+      <c r="G298" s="3">
+        <v>124</v>
+      </c>
+      <c r="H298" s="3">
+        <v>25</v>
+      </c>
+      <c r="I298" s="3">
+        <v>11</v>
+      </c>
+      <c r="J298">
+        <v>5</v>
+      </c>
+      <c r="K298" t="s">
+        <v>65</v>
+      </c>
+      <c r="L298">
+        <v>3</v>
+      </c>
+      <c r="M298" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="299" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A299">
+        <v>2</v>
+      </c>
+      <c r="B299" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C299" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D299" t="s">
+        <v>9</v>
+      </c>
+      <c r="E299" t="s">
+        <v>151</v>
+      </c>
+      <c r="F299" s="2">
+        <v>123</v>
+      </c>
+      <c r="G299" s="3">
+        <v>216</v>
+      </c>
+      <c r="H299" s="3">
+        <v>24</v>
+      </c>
+      <c r="I299" s="3">
+        <v>12</v>
+      </c>
+      <c r="J299">
+        <v>5</v>
+      </c>
+      <c r="K299" t="s">
+        <v>65</v>
+      </c>
+      <c r="L299">
+        <v>3</v>
+      </c>
+      <c r="M299" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="300" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A300">
+        <v>3</v>
+      </c>
+      <c r="B300" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C300" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D300" t="s">
+        <v>9</v>
+      </c>
+      <c r="E300" t="s">
+        <v>58</v>
+      </c>
+      <c r="F300" s="2">
+        <v>126</v>
+      </c>
+      <c r="G300" s="3">
+        <v>180</v>
+      </c>
+      <c r="H300" s="3">
+        <v>23</v>
+      </c>
+      <c r="I300" s="3">
+        <v>8</v>
+      </c>
+      <c r="J300">
+        <v>5</v>
+      </c>
+      <c r="K300" t="s">
+        <v>65</v>
+      </c>
+      <c r="L300">
+        <v>3</v>
+      </c>
+      <c r="M300" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="301" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A301">
+        <v>4</v>
+      </c>
+      <c r="B301" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C301" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="D301" t="s">
+        <v>11</v>
+      </c>
+      <c r="E301" t="s">
+        <v>27</v>
+      </c>
+      <c r="F301" s="2">
+        <v>77</v>
+      </c>
+      <c r="G301" s="3">
+        <v>149</v>
+      </c>
+      <c r="H301" s="3">
+        <v>18</v>
+      </c>
+      <c r="I301" s="3">
+        <v>8</v>
+      </c>
+      <c r="J301">
+        <v>5</v>
+      </c>
+      <c r="K301" t="s">
+        <v>65</v>
+      </c>
+      <c r="L301">
+        <v>3</v>
+      </c>
+      <c r="M301" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="302" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A302">
+        <v>5</v>
+      </c>
+      <c r="B302" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C302" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D302" t="s">
+        <v>7</v>
+      </c>
+      <c r="E302" t="s">
+        <v>13</v>
+      </c>
+      <c r="F302" s="2">
+        <v>72</v>
+      </c>
+      <c r="G302" s="3">
+        <v>93</v>
+      </c>
+      <c r="H302" s="3">
+        <v>15</v>
+      </c>
+      <c r="I302" s="3">
+        <v>9</v>
+      </c>
+      <c r="J302">
+        <v>5</v>
+      </c>
+      <c r="K302" t="s">
+        <v>65</v>
+      </c>
+      <c r="L302">
+        <v>3</v>
+      </c>
+      <c r="M302" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="303" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A303">
+        <v>6</v>
+      </c>
+      <c r="B303" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C303" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D303" t="s">
+        <v>9</v>
+      </c>
+      <c r="E303" t="s">
+        <v>171</v>
+      </c>
+      <c r="F303" s="2">
+        <v>66</v>
+      </c>
+      <c r="G303" s="3">
+        <v>75</v>
+      </c>
+      <c r="H303" s="3">
+        <v>15</v>
+      </c>
+      <c r="I303" s="3">
+        <v>8</v>
+      </c>
+      <c r="J303">
+        <v>5</v>
+      </c>
+      <c r="K303" t="s">
+        <v>65</v>
+      </c>
+      <c r="L303">
+        <v>3</v>
+      </c>
+      <c r="M303" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="304" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A304">
+        <v>7</v>
+      </c>
+      <c r="B304" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C304" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D304" t="s">
+        <v>41</v>
+      </c>
+      <c r="E304" t="s">
+        <v>62</v>
+      </c>
+      <c r="F304" s="2">
+        <v>46</v>
+      </c>
+      <c r="G304" s="3">
+        <v>21</v>
+      </c>
+      <c r="H304" s="3">
+        <v>7</v>
+      </c>
+      <c r="I304" s="3">
+        <v>11</v>
+      </c>
+      <c r="J304">
+        <v>5</v>
+      </c>
+      <c r="K304" t="s">
+        <v>65</v>
+      </c>
+      <c r="L304">
+        <v>3</v>
+      </c>
+      <c r="M304" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="305" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A305">
+        <v>8</v>
+      </c>
+      <c r="B305" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C305" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D305" t="s">
+        <v>12</v>
+      </c>
+      <c r="E305" t="s">
+        <v>42</v>
+      </c>
+      <c r="F305" s="2">
+        <v>39</v>
+      </c>
+      <c r="G305" s="3">
+        <v>15</v>
+      </c>
+      <c r="H305" s="3">
+        <v>7</v>
+      </c>
+      <c r="I305" s="3">
+        <v>10</v>
+      </c>
+      <c r="J305">
+        <v>5</v>
+      </c>
+      <c r="K305" t="s">
+        <v>65</v>
+      </c>
+      <c r="L305">
+        <v>3</v>
+      </c>
+      <c r="M305" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="306" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A306">
+        <v>1</v>
+      </c>
+      <c r="B306" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C306" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="D306" t="s">
+        <v>12</v>
+      </c>
+      <c r="E306" t="s">
+        <v>27</v>
+      </c>
+      <c r="F306" s="2">
+        <v>102</v>
+      </c>
+      <c r="G306" s="3">
+        <v>231</v>
+      </c>
+      <c r="H306" s="3">
+        <v>22</v>
+      </c>
+      <c r="I306" s="3">
+        <v>7</v>
+      </c>
+      <c r="J306">
+        <v>5</v>
+      </c>
+      <c r="K306" t="s">
+        <v>65</v>
+      </c>
+      <c r="L306">
+        <v>4</v>
+      </c>
+      <c r="M306" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="307" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A307">
+        <v>2</v>
+      </c>
+      <c r="B307" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C307" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D307" t="s">
+        <v>12</v>
+      </c>
+      <c r="E307" t="s">
+        <v>27</v>
+      </c>
+      <c r="F307" s="2">
+        <v>88</v>
+      </c>
+      <c r="G307" s="3">
+        <v>149</v>
+      </c>
+      <c r="H307" s="3">
+        <v>20</v>
+      </c>
+      <c r="I307" s="3">
+        <v>9</v>
+      </c>
+      <c r="J307">
+        <v>5</v>
+      </c>
+      <c r="K307" t="s">
+        <v>65</v>
+      </c>
+      <c r="L307">
+        <v>4</v>
+      </c>
+      <c r="M307" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="308" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A308">
+        <v>3</v>
+      </c>
+      <c r="B308" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C308" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D308" t="s">
+        <v>41</v>
+      </c>
+      <c r="E308" t="s">
+        <v>21</v>
+      </c>
+      <c r="F308" s="2">
+        <v>94</v>
+      </c>
+      <c r="G308" s="3">
+        <v>125</v>
+      </c>
+      <c r="H308" s="3">
+        <v>15</v>
+      </c>
+      <c r="I308" s="3">
+        <v>14</v>
+      </c>
+      <c r="J308">
+        <v>5</v>
+      </c>
+      <c r="K308" t="s">
+        <v>65</v>
+      </c>
+      <c r="L308">
+        <v>4</v>
+      </c>
+      <c r="M308" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="309" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A309">
+        <v>4</v>
+      </c>
+      <c r="B309" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C309" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D309" t="s">
+        <v>41</v>
+      </c>
+      <c r="E309" t="s">
+        <v>62</v>
+      </c>
+      <c r="F309" s="2">
+        <v>82</v>
+      </c>
+      <c r="G309" s="3">
+        <v>75</v>
+      </c>
+      <c r="H309" s="3">
+        <v>17</v>
+      </c>
+      <c r="I309" s="3">
+        <v>11</v>
+      </c>
+      <c r="J309">
+        <v>5</v>
+      </c>
+      <c r="K309" t="s">
+        <v>65</v>
+      </c>
+      <c r="L309">
+        <v>4</v>
+      </c>
+      <c r="M309" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="310" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A310">
+        <v>5</v>
+      </c>
+      <c r="B310" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C310" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="D310" t="s">
+        <v>7</v>
+      </c>
+      <c r="E310" t="s">
+        <v>18</v>
+      </c>
+      <c r="F310" s="2">
+        <v>86</v>
+      </c>
+      <c r="G310" s="3">
+        <v>94</v>
+      </c>
+      <c r="H310" s="3">
+        <v>15</v>
+      </c>
+      <c r="I310" s="3">
+        <v>12</v>
+      </c>
+      <c r="J310">
+        <v>5</v>
+      </c>
+      <c r="K310" t="s">
+        <v>65</v>
+      </c>
+      <c r="L310">
+        <v>4</v>
+      </c>
+      <c r="M310" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="311" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A311">
+        <v>6</v>
+      </c>
+      <c r="B311" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C311" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D311" t="s">
+        <v>11</v>
+      </c>
+      <c r="E311" t="s">
+        <v>149</v>
+      </c>
+      <c r="F311" s="2">
+        <v>79</v>
+      </c>
+      <c r="G311" s="3">
+        <v>49</v>
+      </c>
+      <c r="H311" s="3">
+        <v>15</v>
+      </c>
+      <c r="I311" s="3">
+        <v>11</v>
+      </c>
+      <c r="J311">
+        <v>5</v>
+      </c>
+      <c r="K311" t="s">
+        <v>65</v>
+      </c>
+      <c r="L311">
+        <v>4</v>
+      </c>
+      <c r="M311" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="312" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A312">
+        <v>7</v>
+      </c>
+      <c r="B312" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C312" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D312" t="s">
+        <v>11</v>
+      </c>
+      <c r="E312" t="s">
+        <v>27</v>
+      </c>
+      <c r="F312" s="2">
+        <v>65</v>
+      </c>
+      <c r="G312" s="3">
+        <v>90</v>
+      </c>
+      <c r="H312" s="3">
+        <v>14</v>
+      </c>
+      <c r="I312" s="3">
+        <v>10</v>
+      </c>
+      <c r="J312">
+        <v>5</v>
+      </c>
+      <c r="K312" t="s">
+        <v>65</v>
+      </c>
+      <c r="L312">
+        <v>4</v>
+      </c>
+      <c r="M312" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="313" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A313">
+        <v>8</v>
+      </c>
+      <c r="B313" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C313" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D313" t="s">
+        <v>7</v>
+      </c>
+      <c r="E313" t="s">
+        <v>18</v>
+      </c>
+      <c r="F313" s="2">
+        <v>41</v>
+      </c>
+      <c r="G313" s="3">
+        <v>16</v>
+      </c>
+      <c r="H313" s="3">
+        <v>7</v>
+      </c>
+      <c r="I313" s="3">
+        <v>9</v>
+      </c>
+      <c r="J313">
+        <v>5</v>
+      </c>
+      <c r="K313" t="s">
+        <v>65</v>
+      </c>
+      <c r="L313">
+        <v>4</v>
+      </c>
+      <c r="M313" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="314" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A314">
+        <v>1</v>
+      </c>
+      <c r="B314" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C314" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D314" t="s">
+        <v>59</v>
+      </c>
+      <c r="E314" t="s">
+        <v>94</v>
+      </c>
+      <c r="F314" s="2">
+        <v>123</v>
+      </c>
+      <c r="G314" s="3">
+        <v>120</v>
+      </c>
+      <c r="H314" s="3">
+        <v>21</v>
+      </c>
+      <c r="I314" s="3">
+        <v>10</v>
+      </c>
+      <c r="J314">
+        <v>5</v>
+      </c>
+      <c r="K314" t="s">
+        <v>65</v>
+      </c>
+      <c r="L314">
+        <v>5</v>
+      </c>
+      <c r="M314" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="315" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A315">
+        <v>2</v>
+      </c>
+      <c r="B315" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C315" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D315" t="s">
+        <v>11</v>
+      </c>
+      <c r="E315" t="s">
+        <v>27</v>
+      </c>
+      <c r="F315" s="2">
+        <v>96</v>
+      </c>
+      <c r="G315" s="3">
+        <v>125</v>
+      </c>
+      <c r="H315" s="3">
+        <v>22</v>
+      </c>
+      <c r="I315" s="3">
+        <v>9</v>
+      </c>
+      <c r="J315">
+        <v>5</v>
+      </c>
+      <c r="K315" t="s">
+        <v>65</v>
+      </c>
+      <c r="L315">
+        <v>5</v>
+      </c>
+      <c r="M315" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="316" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A316">
+        <v>3</v>
+      </c>
+      <c r="B316" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C316" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D316" t="s">
+        <v>9</v>
+      </c>
+      <c r="E316" t="s">
+        <v>21</v>
+      </c>
+      <c r="F316" s="2">
+        <v>99</v>
+      </c>
+      <c r="G316" s="3">
+        <v>151</v>
+      </c>
+      <c r="H316" s="3">
+        <v>20</v>
+      </c>
+      <c r="I316" s="3">
+        <v>11</v>
+      </c>
+      <c r="J316">
+        <v>5</v>
+      </c>
+      <c r="K316" t="s">
+        <v>65</v>
+      </c>
+      <c r="L316">
+        <v>5</v>
+      </c>
+      <c r="M316" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="317" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A317">
+        <v>4</v>
+      </c>
+      <c r="B317" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C317" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D317" t="s">
+        <v>12</v>
+      </c>
+      <c r="E317" t="s">
+        <v>178</v>
+      </c>
+      <c r="F317" s="2">
+        <v>102</v>
+      </c>
+      <c r="G317" s="3">
+        <v>141</v>
+      </c>
+      <c r="H317" s="3">
+        <v>19</v>
+      </c>
+      <c r="I317" s="3">
+        <v>9</v>
+      </c>
+      <c r="J317">
+        <v>5</v>
+      </c>
+      <c r="K317" t="s">
+        <v>65</v>
+      </c>
+      <c r="L317">
+        <v>5</v>
+      </c>
+      <c r="M317" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="318" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A318">
+        <v>5</v>
+      </c>
+      <c r="B318" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C318" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D318" t="s">
+        <v>12</v>
+      </c>
+      <c r="E318" t="s">
+        <v>58</v>
+      </c>
+      <c r="F318" s="2">
+        <v>63</v>
+      </c>
+      <c r="G318" s="3">
+        <v>124</v>
+      </c>
+      <c r="H318" s="3">
+        <v>15</v>
+      </c>
+      <c r="I318" s="3">
+        <v>8</v>
+      </c>
+      <c r="J318">
+        <v>5</v>
+      </c>
+      <c r="K318" t="s">
+        <v>65</v>
+      </c>
+      <c r="L318">
+        <v>5</v>
+      </c>
+      <c r="M318" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="319" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A319">
+        <v>6</v>
+      </c>
+      <c r="B319" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C319" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D319" t="s">
+        <v>9</v>
+      </c>
+      <c r="E319" t="s">
+        <v>176</v>
+      </c>
+      <c r="F319" s="2">
+        <v>75</v>
+      </c>
+      <c r="G319" s="3">
+        <v>78</v>
+      </c>
+      <c r="H319" s="3">
+        <v>12</v>
+      </c>
+      <c r="I319" s="3">
+        <v>10</v>
+      </c>
+      <c r="J319">
+        <v>5</v>
+      </c>
+      <c r="K319" t="s">
+        <v>65</v>
+      </c>
+      <c r="L319">
+        <v>5</v>
+      </c>
+      <c r="M319" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="320" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A320">
+        <v>7</v>
+      </c>
+      <c r="B320" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C320" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D320" t="s">
+        <v>41</v>
+      </c>
+      <c r="E320" t="s">
+        <v>156</v>
+      </c>
+      <c r="F320" s="2">
+        <v>46</v>
+      </c>
+      <c r="G320" s="3">
+        <v>42</v>
+      </c>
+      <c r="H320" s="3">
+        <v>10</v>
+      </c>
+      <c r="I320" s="3">
+        <v>9</v>
+      </c>
+      <c r="J320">
+        <v>5</v>
+      </c>
+      <c r="K320" t="s">
+        <v>65</v>
+      </c>
+      <c r="L320">
+        <v>5</v>
+      </c>
+      <c r="M320" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="321" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A321">
+        <v>8</v>
+      </c>
+      <c r="B321" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C321" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="D321" t="s">
+        <v>11</v>
+      </c>
+      <c r="E321" t="s">
+        <v>21</v>
+      </c>
+      <c r="F321" s="2">
+        <v>48</v>
+      </c>
+      <c r="G321" s="3">
+        <v>12</v>
+      </c>
+      <c r="H321" s="3">
+        <v>6</v>
+      </c>
+      <c r="I321" s="3">
+        <v>11</v>
+      </c>
+      <c r="J321">
+        <v>5</v>
+      </c>
+      <c r="K321" t="s">
+        <v>65</v>
+      </c>
+      <c r="L321">
+        <v>5</v>
+      </c>
+      <c r="M321" t="s">
         <v>63</v>
       </c>
     </row>
@@ -10993,8 +14302,8 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1" xr:uid="{C4A33699-B861-4CDE-859A-34709F1ACEE7}">
       <formula1>"魔坦刺,扶桑法刺,扶桑群雄刺,七射,稷下战,法奶,轻战守约,魔种(有天赋),攻辅射,蜀国,弟弟射,魔种(无天赋),九战,攻辅蛋"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E1048576" xr:uid="{285C689A-B700-4D5B-9BA9-A6E5ACD32491}">
-      <formula1>"魔坦刺,扶桑法刺,扶桑群雄刺,七射,稷下战,法奶,轻战守约,魔种(有天赋),攻辅射,蜀国,弟弟射,魔种(无天赋),九战,攻辅蛋,扶桑法,魏战,扶桑群雄法刺,吴国攻辅射,稷下攻辅射,封神攻辅射,坦法,弟妹法,尧天攻辅射,长城攻辅射"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E1048576" xr:uid="{E38A29DF-2802-4753-B902-8CC4AF0BB8DA}">
+      <formula1>"魔坦刺,长城战,扶桑刺,扶桑法刺,扶桑群雄刺,弟弟蜀,七射,稷下战,法奶,轻战守约,魔种(有天赋),攻辅射,蜀国,弟弟射,魔种(无天赋),九战,攻辅蛋,扶桑法,魏战,扶桑群雄法刺,吴国攻辅射,稷下攻辅射,封神攻辅射,坦法,弟妹法,尧天攻辅射,长城攻辅射"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>